<commit_message>
several minor fixes mainly around handling floating point
</commit_message>
<xml_diff>
--- a/jumpstart/metameta.xlsx
+++ b/jumpstart/metameta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erickohlenberg/src/jumpstart/jumpstart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F9F002-7E7F-C64F-A88C-2E972788A08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F755CECD-F705-8444-86C4-639F44DF100C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8380" yWindow="15260" windowWidth="37200" windowHeight="24540" xr2:uid="{17A214B1-8C09-2A44-82CB-BCF2101EEBF1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19440" activeTab="1" xr2:uid="{17A214B1-8C09-2A44-82CB-BCF2101EEBF1}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaData Structure" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="89">
   <si>
     <t>TABLE_CATALOG</t>
   </si>
@@ -283,6 +283,27 @@
   </si>
   <si>
     <t>The POSTGRES data type.  Current supported types are BIGINT, VARCHAR, NUMERIC(18,4), TIMESTAMP, INTEGER, and DATE</t>
+  </si>
+  <si>
+    <t>Input Type</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>TextArea</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>{"$dt", "$it"},</t>
   </si>
 </sst>
 </file>
@@ -313,7 +334,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -336,11 +357,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -351,6 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,7 +718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F7762C7-9780-FE4B-AE3C-5BD12F6D9DC8}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -849,10 +880,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92ABDC4B-EC08-8A43-A60C-80EE3A41121B}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -865,7 +896,7 @@
     <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -887,8 +918,17 @@
       <c r="I1" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -907,8 +947,18 @@
       <c r="I2" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N2" t="str">
+        <f>SUBSTITUTE(LOWER(SUBSTITUTE($N$1,"$dt", K2)), "$it",L2)</f>
+        <v>{"integer", "Number"},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -927,8 +977,18 @@
       <c r="I3" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N20" si="0">SUBSTITUTE(LOWER(SUBSTITUTE($N$1,"$dt", K3)), "$it",L3)</f>
+        <v>{"bigint", "Number"},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -947,8 +1007,18 @@
       <c r="I4" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" si="0"/>
+        <v>{"smallint", "Number"},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -967,8 +1037,18 @@
       <c r="I5" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="0"/>
+        <v>{"serial", "Number"},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
@@ -984,8 +1064,18 @@
       <c r="I6" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="0"/>
+        <v>{"bigserial", "Number"},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
         <v>31</v>
       </c>
@@ -1001,109 +1091,249 @@
       <c r="I7" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="0"/>
+        <v>{"boolean", "Radio"},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H8" s="1" t="s">
         <v>70</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="0"/>
+        <v>{"char", "Text"},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H9" s="1" t="s">
         <v>47</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="0"/>
+        <v>{"varchar", "Text"},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H10" s="1" t="s">
         <v>71</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="0"/>
+        <v>{"text", "TextArea"},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H11" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="0"/>
+        <v>{"date", "Date"},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H12" s="1" t="s">
         <v>51</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="0"/>
+        <v>{"timestamp", "Date"},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H13" s="1" t="s">
         <v>72</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="0"/>
+        <v>{"timestamptz", "Date"},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H14" s="1" t="s">
         <v>73</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="0"/>
+        <v>{"real", "Number"},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H15" s="1" t="s">
         <v>74</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="0"/>
+        <v>{"double precision", "Number"},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H16" s="1" t="s">
         <v>75</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="K16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="0"/>
+        <v>{"numeric", "Number"},</v>
+      </c>
+    </row>
+    <row r="17" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H17" s="1" t="s">
         <v>76</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="K17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="0"/>
+        <v>{"json", "TextArea"},</v>
+      </c>
+    </row>
+    <row r="18" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H18" s="1" t="s">
         <v>77</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="K18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="0"/>
+        <v>{"uuid", "Text"},</v>
+      </c>
+    </row>
+    <row r="19" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H19" s="1" t="s">
         <v>78</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="K19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="0"/>
+        <v>{"bytea", "Text"},</v>
+      </c>
+    </row>
+    <row r="20" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H20" s="1" t="s">
         <v>79</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>60</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="0"/>
+        <v>{"xml", "Text"},</v>
       </c>
     </row>
   </sheetData>
@@ -1111,5 +1341,6 @@
     <sortCondition ref="C2:C85"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>